<commit_message>
create all the endpoints on real app
</commit_message>
<xml_diff>
--- a/data/dataset_RAG.xlsx
+++ b/data/dataset_RAG.xlsx
@@ -775,7 +775,7 @@
     <col min="7" max="7" style="7" width="8.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -798,7 +798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -821,7 +821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="87">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="89.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>

</xml_diff>